<commit_message>
finished 1st iteration of results
</commit_message>
<xml_diff>
--- a/src/integration/data/FormatoExcelImportacion.xlsx
+++ b/src/integration/data/FormatoExcelImportacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Huerta\Documents\nhuerta\Proyectos\zeroco\BackEnd\src\integration\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{365CB726-142B-4504-8592-689E966D92BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E774B885-632A-4044-B084-29BC905980AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D33B081F-D4DC-4846-A063-7103A2C188E6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D33B081F-D4DC-4846-A063-7103A2C188E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="240">
   <si>
     <t>Alcance</t>
   </si>
@@ -697,9 +697,6 @@
   </si>
   <si>
     <t xml:space="preserve">Fuentes fijas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medio terrestres </t>
   </si>
   <si>
     <t>Gas licuado</t>
@@ -767,7 +764,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -871,7 +868,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -904,12 +901,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -920,20 +911,20 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1253,7 +1244,7 @@
   <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1262,7 +1253,7 @@
     <col min="2" max="2" width="57.81640625" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.90625" style="10" customWidth="1"/>
     <col min="4" max="4" width="43.81640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.81640625" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.26953125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10.90625" style="2"/>
@@ -1281,20 +1272,20 @@
       <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="5" t="s">
         <v>208</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="17" t="s">
         <v>209</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>216</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1310,7 +1301,7 @@
       <c r="D2" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="10">
         <f>23210/1000</f>
         <v>23.21</v>
       </c>
@@ -1331,13 +1322,13 @@
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>220</v>
+      <c r="C3" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="10">
         <f>3580/1000</f>
         <v>3.58</v>
       </c>
@@ -1364,7 +1355,7 @@
       <c r="D4" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <f>1129243/1000</f>
         <v>1129.2429999999999</v>
       </c>
@@ -1375,7 +1366,7 @@
         <v>215</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1391,7 +1382,7 @@
       <c r="D5" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <f>8951/1000</f>
         <v>8.9510000000000005</v>
       </c>
@@ -1418,7 +1409,7 @@
       <c r="D6" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <f>105022/1000</f>
         <v>105.02200000000001</v>
       </c>
@@ -1429,7 +1420,7 @@
         <v>215</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1443,9 +1434,9 @@
         <v>22</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="E7" s="13">
+        <v>220</v>
+      </c>
+      <c r="E7" s="10">
         <f>21920/1000</f>
         <v>21.92</v>
       </c>
@@ -1472,7 +1463,7 @@
       <c r="D8" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <f>135132/1000</f>
         <v>135.13200000000001</v>
       </c>
@@ -1483,7 +1474,7 @@
         <v>215</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1499,7 +1490,7 @@
       <c r="D9" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <f>700/1000</f>
         <v>0.7</v>
       </c>
@@ -1524,9 +1515,9 @@
         <v>22</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="E10" s="13">
+        <v>221</v>
+      </c>
+      <c r="E10" s="10">
         <f>5221203/1000</f>
         <v>5221.2030000000004</v>
       </c>
@@ -1553,7 +1544,7 @@
       <c r="D11" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="10">
         <f>756989/1000</f>
         <v>756.98900000000003</v>
       </c>
@@ -1564,7 +1555,7 @@
         <v>215</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1580,7 +1571,7 @@
       <c r="D12" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="10">
         <f>3664514/1000</f>
         <v>3664.5140000000001</v>
       </c>
@@ -1607,7 +1598,7 @@
       <c r="D13" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="10">
         <f>35600/1000</f>
         <v>35.6</v>
       </c>
@@ -1632,9 +1623,9 @@
         <v>49</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="E14" s="13">
+        <v>221</v>
+      </c>
+      <c r="E14" s="10">
         <f>240434/1000</f>
         <v>240.434</v>
       </c>
@@ -1661,7 +1652,7 @@
       <c r="D15" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="10">
         <f>1191116/1000</f>
         <v>1191.116</v>
       </c>
@@ -1675,27 +1666,27 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="20" t="s">
+    <row r="16" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18">
         <f>15626/1000</f>
         <v>15.625999999999999</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="I16" s="14">
+      <c r="F16" s="18"/>
+      <c r="G16" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="I16" s="12">
         <v>1810</v>
       </c>
     </row>
@@ -1712,7 +1703,7 @@
       <c r="D17" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="10">
         <v>709</v>
       </c>
       <c r="F17" s="10" t="s">
@@ -1722,7 +1713,7 @@
         <v>215</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1738,7 +1729,7 @@
       <c r="D18" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="10">
         <v>90</v>
       </c>
       <c r="F18" s="10" t="s">
@@ -1748,7 +1739,7 @@
         <v>215</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1764,7 +1755,7 @@
       <c r="D19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="10">
         <v>136</v>
       </c>
       <c r="F19" s="10" t="s">
@@ -1774,7 +1765,7 @@
         <v>215</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1785,17 +1776,17 @@
         <v>13</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="E20" s="13">
+        <v>227</v>
+      </c>
+      <c r="E20" s="10">
         <f>27914/1000</f>
         <v>27.914000000000001</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>215</v>
@@ -1812,17 +1803,17 @@
         <v>13</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="E21" s="13">
+        <v>227</v>
+      </c>
+      <c r="E21" s="10">
         <f>26738/1000</f>
         <v>26.738</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>215</v>
@@ -1839,23 +1830,23 @@
         <v>13</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="E22" s="13">
+        <v>231</v>
+      </c>
+      <c r="E22" s="10">
         <f>4525740/1000</f>
         <v>4525.74</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>215</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1866,17 +1857,17 @@
         <v>13</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="E23" s="13">
+        <v>231</v>
+      </c>
+      <c r="E23" s="10">
         <f>35683/1000</f>
         <v>35.683</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>215</v>
@@ -1893,17 +1884,17 @@
         <v>13</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="E24" s="13">
+        <v>231</v>
+      </c>
+      <c r="E24" s="10">
         <f>21344/1000</f>
         <v>21.344000000000001</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>215</v>
@@ -1920,23 +1911,23 @@
         <v>13</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="E25" s="13">
+        <v>231</v>
+      </c>
+      <c r="E25" s="10">
         <f>16327818/1000</f>
         <v>16327.817999999999</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>215</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1952,7 +1943,7 @@
       <c r="D26" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="10">
         <f>22773/1000</f>
         <v>22.773</v>
       </c>
@@ -1974,22 +1965,22 @@
         <v>16</v>
       </c>
       <c r="C27" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="E27" s="13">
+      <c r="E27" s="10">
         <v>4203498</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>215</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -2000,16 +1991,16 @@
         <v>16</v>
       </c>
       <c r="C28" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="D28" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="E28" s="13">
+      <c r="E28" s="10">
         <v>119043744</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>215</v>
@@ -2018,39 +2009,39 @@
         <v>217</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="I29" s="14"/>
-    </row>
-    <row r="30" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="H30" s="14" t="s">
+    <row r="29" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="H29" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="I30" s="14"/>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
@@ -2065,7 +2056,7 @@
       <c r="D31" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="10">
         <f>23308/1000</f>
         <v>23.308</v>
       </c>
@@ -2092,7 +2083,7 @@
       <c r="D32" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="10">
         <f>212000/1000</f>
         <v>212</v>
       </c>
@@ -2103,7 +2094,7 @@
         <v>215</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -2119,7 +2110,7 @@
       <c r="D33" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="10">
         <f>5470/1000</f>
         <v>5.47</v>
       </c>
@@ -2130,25 +2121,25 @@
         <v>215</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="H34" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="I34" s="14"/>
+    </row>
+    <row r="34" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="I34" s="12"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
@@ -2163,7 +2154,7 @@
       <c r="D35" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="10">
         <f>32984/1000</f>
         <v>32.984000000000002</v>
       </c>
@@ -2190,7 +2181,7 @@
       <c r="D36" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="10">
         <f>3100/1000</f>
         <v>3.1</v>
       </c>
@@ -2201,7 +2192,7 @@
         <v>215</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -2217,7 +2208,7 @@
       <c r="D37" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="10">
         <f>5000/1000</f>
         <v>5</v>
       </c>
@@ -2244,7 +2235,7 @@
       <c r="D38" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="10">
         <f>1871000/1000</f>
         <v>1871</v>
       </c>
@@ -2255,25 +2246,25 @@
         <v>215</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="H39" s="14" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="H39" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="I39" s="14"/>
+      <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
@@ -2288,7 +2279,7 @@
       <c r="D40" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="10">
         <f>1435000/1000</f>
         <v>1435</v>
       </c>
@@ -2299,7 +2290,7 @@
         <v>215</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -2315,7 +2306,7 @@
       <c r="D41" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="10">
         <f>38000/1000</f>
         <v>38</v>
       </c>
@@ -2326,7 +2317,7 @@
         <v>215</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -2342,7 +2333,7 @@
       <c r="D42" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="10">
         <f>21599/1000</f>
         <v>21.599</v>
       </c>
@@ -2369,7 +2360,7 @@
       <c r="D43" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="10">
         <f>46584/1000</f>
         <v>46.584000000000003</v>
       </c>
@@ -2396,7 +2387,7 @@
       <c r="D44" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="10">
         <f>697475/1000</f>
         <v>697.47500000000002</v>
       </c>
@@ -2417,7 +2408,7 @@
       <c r="B45" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="13">
+      <c r="E45" s="10">
         <f>176231/1000</f>
         <v>176.23099999999999</v>
       </c>
@@ -2438,7 +2429,7 @@
       <c r="B46" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E46" s="13">
+      <c r="E46" s="10">
         <f>7620/1000</f>
         <v>7.62</v>
       </c>
@@ -2446,7 +2437,7 @@
         <v>215</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I46" s="2">
         <v>400</v>
@@ -2459,7 +2450,7 @@
       <c r="B47" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E47" s="13">
+      <c r="E47" s="10">
         <f>138/1000</f>
         <v>0.13800000000000001</v>
       </c>
@@ -2480,7 +2471,7 @@
       <c r="B48" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E48" s="13">
+      <c r="E48" s="10">
         <f>18482/1000</f>
         <v>18.481999999999999</v>
       </c>
@@ -2501,7 +2492,7 @@
       <c r="B49" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E49" s="10">
         <f>493/1000</f>
         <v>0.49299999999999999</v>
       </c>
@@ -2509,7 +2500,7 @@
         <v>215</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I49" s="2">
         <v>2000</v>
@@ -2528,7 +2519,7 @@
       <c r="D50" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E50" s="13">
+      <c r="E50" s="10">
         <f>10463/1000</f>
         <v>10.462999999999999</v>
       </c>
@@ -2539,7 +2530,7 @@
         <v>215</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
@@ -2555,7 +2546,7 @@
       <c r="D51" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E51" s="13">
+      <c r="E51" s="10">
         <f>408687/1000</f>
         <v>408.68700000000001</v>
       </c>
@@ -2582,7 +2573,7 @@
       <c r="D52" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="13">
+      <c r="E52" s="10">
         <f>164080/1000</f>
         <v>164.08</v>
       </c>
@@ -2593,7 +2584,7 @@
         <v>215</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
@@ -2603,7 +2594,7 @@
       <c r="B53" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E53" s="13">
+      <c r="E53" s="10">
         <f>491610/1000</f>
         <v>491.61</v>
       </c>
@@ -2611,7 +2602,7 @@
         <v>215</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I53" s="2">
         <v>20</v>
@@ -2624,7 +2615,7 @@
       <c r="B54" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E54" s="13">
+      <c r="E54" s="10">
         <f>7102106/1000</f>
         <v>7102.1059999999998</v>
       </c>
@@ -2645,7 +2636,7 @@
       <c r="B55" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E55" s="13">
+      <c r="E55" s="10">
         <f>13977776/1000</f>
         <v>13977.776</v>
       </c>
@@ -2653,7 +2644,7 @@
         <v>215</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I55" s="2">
         <v>20</v>
@@ -2672,7 +2663,7 @@
       <c r="D56" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E56" s="13">
+      <c r="E56" s="10">
         <f>130360/1000</f>
         <v>130.36000000000001</v>
       </c>
@@ -2683,7 +2674,7 @@
         <v>215</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
@@ -2699,7 +2690,7 @@
       <c r="D57" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E57" s="13">
+      <c r="E57" s="10">
         <f>2117953/1000</f>
         <v>2117.953</v>
       </c>
@@ -2726,7 +2717,7 @@
       <c r="D58" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E58" s="13">
+      <c r="E58" s="10">
         <f>350076/1000</f>
         <v>350.07600000000002</v>
       </c>
@@ -2737,7 +2728,7 @@
         <v>215</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
@@ -2753,7 +2744,7 @@
       <c r="D59" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E59" s="13">
+      <c r="E59" s="10">
         <v>23568498</v>
       </c>
       <c r="F59" s="10" t="s">
@@ -2763,25 +2754,25 @@
         <v>215</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="H60" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="I60" s="14"/>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="I60" s="12"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="s">
@@ -2796,7 +2787,7 @@
       <c r="D61" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E61" s="13">
+      <c r="E61" s="10">
         <v>302936543</v>
       </c>
       <c r="F61" s="10" t="s">
@@ -2806,7 +2797,7 @@
         <v>215</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
@@ -2822,7 +2813,7 @@
       <c r="D62" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="E62" s="13">
+      <c r="E62" s="10">
         <v>4047625</v>
       </c>
       <c r="F62" s="10" t="s">
@@ -2832,7 +2823,7 @@
         <v>215</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -2848,7 +2839,7 @@
       <c r="D63" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="E63" s="13">
+      <c r="E63" s="10">
         <v>189545979</v>
       </c>
       <c r="F63" s="10" t="s">
@@ -2858,7 +2849,7 @@
         <v>215</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
@@ -2874,7 +2865,7 @@
       <c r="D64" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="E64" s="13">
+      <c r="E64" s="10">
         <v>74706163</v>
       </c>
       <c r="F64" s="10" t="s">
@@ -2884,7 +2875,7 @@
         <v>215</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
@@ -2900,7 +2891,7 @@
       <c r="D65" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="E65" s="13">
+      <c r="E65" s="10">
         <v>36660864</v>
       </c>
       <c r="F65" s="10" t="s">
@@ -2910,7 +2901,7 @@
         <v>215</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
@@ -2926,7 +2917,7 @@
       <c r="D66" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="E66" s="13">
+      <c r="E66" s="10">
         <v>1141648</v>
       </c>
       <c r="F66" s="10" t="s">
@@ -2952,7 +2943,7 @@
       <c r="D67" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="E67" s="13">
+      <c r="E67" s="10">
         <v>13879453</v>
       </c>
       <c r="F67" s="10" t="s">
@@ -2962,7 +2953,7 @@
         <v>215</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
@@ -2978,7 +2969,7 @@
       <c r="D68" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="E68" s="13">
+      <c r="E68" s="10">
         <v>714315</v>
       </c>
       <c r="F68" s="10" t="s">
@@ -3004,7 +2995,7 @@
       <c r="D69" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="E69" s="13">
+      <c r="E69" s="10">
         <v>498105</v>
       </c>
       <c r="F69" s="10" t="s">
@@ -3115,11 +3106,11 @@
       <c r="F1" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>236</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -3287,14 +3278,14 @@
       <c r="D10" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="G10" s="15">
+      <c r="E10" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="G10" s="13">
         <v>0.39069999999999999</v>
       </c>
-      <c r="H10" s="15" t="s">
-        <v>238</v>
+      <c r="H10" s="13" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -3307,14 +3298,14 @@
       <c r="D11" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="G11" s="15">
+      <c r="E11" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="G11" s="13">
         <v>0.72446767990114092</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>238</v>
+      <c r="H11" s="13" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -3327,14 +3318,14 @@
       <c r="D12" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="G12" s="15">
+      <c r="E12" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="G12" s="13">
         <v>0.59281777811558378</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>238</v>
+      <c r="H12" s="13" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -3344,14 +3335,14 @@
       <c r="D13" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="G13" s="18">
+      <c r="E13" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G13" s="16">
         <v>1.8120000000000001</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>238</v>
+      <c r="H13" s="13" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -3361,14 +3352,14 @@
       <c r="D14" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="G14" s="18">
+      <c r="E14" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G14" s="16">
         <v>1.8120000000000001</v>
       </c>
-      <c r="H14" s="15" t="s">
-        <v>238</v>
+      <c r="H14" s="13" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -3378,14 +3369,14 @@
       <c r="D15" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="G15" s="18">
+      <c r="E15" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G15" s="16">
         <v>1.8120000000000001</v>
       </c>
-      <c r="H15" s="15" t="s">
-        <v>238</v>
+      <c r="H15" s="13" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -3813,8 +3804,8 @@
       </c>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C69" s="14" t="s">
-        <v>230</v>
+      <c r="C69" s="12" t="s">
+        <v>229</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>176</v>
@@ -4236,33 +4227,33 @@
       </c>
     </row>
     <row r="153" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D153" s="14" t="s">
+      <c r="D153" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="154" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D154" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="155" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D155" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="156" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D156" s="12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="157" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D157" s="12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D154" s="14" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D155" s="14" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D156" s="14" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D157" s="14" t="s">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D158" s="12" t="s">
         <v>233</v>
-      </c>
-    </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D158" s="14" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>